<commit_message>
Create contentTable fixes #1
とりあえず、テーブルを表示させるところまで編集した
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="シート1" sheetId="1" r:id="rId4"/>
+    <sheet name="appleID" sheetId="1" r:id="rId4"/>
     <sheet name="シート2" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
@@ -23,7 +23,7 @@
     <t>内容</t>
   </si>
   <si>
-    <t>Docomo</t>
+    <t>appleID</t>
   </si>
   <si>
     <t>testContent1</t>
@@ -58,7 +58,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -78,11 +78,6 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="ＭＳ Ｐゴシック"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -260,7 +255,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -322,37 +317,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,9 +1526,7 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1585,20 +1548,20 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="A2" s="21">
+      <c r="A2" s="6">
         <v>44613</v>
       </c>
-      <c r="B2" t="s" s="22">
+      <c r="B2" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="23">
+      <c r="C2" t="s" s="8">
         <v>4</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="18" customHeight="1">
-      <c r="A3" s="25">
+      <c r="A3" s="10">
         <v>44716</v>
       </c>
       <c r="B3" t="s" s="11">
@@ -1611,59 +1574,59 @@
       <c r="E3" s="13"/>
     </row>
     <row r="4" ht="18" customHeight="1">
-      <c r="A4" s="25">
+      <c r="A4" s="10">
         <v>44782</v>
       </c>
-      <c r="B4" t="s" s="26">
+      <c r="B4" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="27">
+      <c r="C4" t="s" s="15">
         <v>8</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="29"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="29"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="29"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" ht="18" customHeight="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
template.js 変更途中 fixes #2
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -106,7 +106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -249,13 +249,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -298,26 +328,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1469,44 +1505,74 @@
       <c r="E4" s="16"/>
     </row>
     <row r="5" ht="17.5" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="10">
+        <v>44778</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>4</v>
+      </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" ht="17.5" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="10">
+        <v>44809</v>
+      </c>
+      <c r="B6" t="s" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>6</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" ht="17.5" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="10">
+        <v>44843</v>
+      </c>
+      <c r="B7" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="15">
+        <v>8</v>
+      </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" ht="17.5" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="16"/>
+      <c r="A8" s="10">
+        <v>44882</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s" s="8">
+        <v>4</v>
+      </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" ht="17.5" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="13"/>
+      <c r="A9" s="10">
+        <v>44900</v>
+      </c>
+      <c r="B9" t="s" s="11">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s" s="12">
+        <v>6</v>
+      </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" ht="17.5" customHeight="1">
       <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
@@ -1577,10 +1643,10 @@
       <c r="A4" s="10">
         <v>44782</v>
       </c>
-      <c r="B4" t="s" s="14">
+      <c r="B4" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="15">
+      <c r="C4" t="s" s="19">
         <v>8</v>
       </c>
       <c r="D4" s="16"/>
@@ -1588,42 +1654,42 @@
     </row>
     <row r="5" ht="18" customHeight="1">
       <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" ht="18" customHeight="1">
       <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" ht="18" customHeight="1">
       <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" ht="18" customHeight="1">
       <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>

</xml_diff>